<commit_message>
More zoomed in coordinates and experimentation with 3D
</commit_message>
<xml_diff>
--- a/track-map/sample.xlsx
+++ b/track-map/sample.xlsx
@@ -20,9 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>latitudelongitude</t>
+  </si>
+  <si>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>longitude</t>
   </si>
   <si>
     <t>latitude</t>
@@ -103,7 +109,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="34">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -144,11 +150,14 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -183,6 +192,9 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -511,10 +523,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
Worked on red dot adding mechanism
-Worked on reconstructing red dots for the map
</commit_message>
<xml_diff>
--- a/track-map/sample.xlsx
+++ b/track-map/sample.xlsx
@@ -20,9 +20,63 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>latitudelongitude</t>
+  </si>
+  <si>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>longitude</t>
+  </si>
+  <si>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>longitude</t>
+  </si>
+  <si>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>longitude</t>
+  </si>
+  <si>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>longitude</t>
+  </si>
+  <si>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>longitude</t>
+  </si>
+  <si>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>longitude</t>
+  </si>
+  <si>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>longitude</t>
+  </si>
+  <si>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>longitude</t>
+  </si>
+  <si>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>longitude</t>
   </si>
   <si>
     <t>latitude</t>
@@ -109,7 +163,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="37">
+  <borders count="64">
     <border>
       <left/>
       <right/>
@@ -153,11 +207,38 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -195,6 +276,33 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="42" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="43" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="44" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="45" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="46" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="47" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="48" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="49" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="50" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="51" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="52" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="53" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="54" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="55" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="56" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="57" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="58" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="59" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="60" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="61" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="62" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="63" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,7 +617,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="M7" sqref="M7"/>
@@ -523,58 +631,98 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>33.777483298660243</v>
+        <v>33.77757633306333</v>
       </c>
       <c r="B2" s="0">
-        <v>-84.400169254656859</v>
+        <v>-84.399890863953885</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>33.77697404011063</v>
+        <v>33.777620190061235</v>
       </c>
       <c r="B3" s="0">
-        <v>-84.399908440834153</v>
+        <v>-84.399819713374711</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>33.776987495858059</v>
+        <v>33.777615538562522</v>
       </c>
       <c r="B4" s="0">
-        <v>-84.399837298254127</v>
+        <v>-84.399861284499607</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>33.777054774563545</v>
+        <v>33.777547759552618</v>
       </c>
       <c r="B5" s="0">
-        <v>-84.399869635790495</v>
+        <v>-84.399821312264123</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>33.777069575871671</v>
+        <v>33.777569023561483</v>
       </c>
       <c r="B6" s="0">
-        <v>-84.399966648399598</v>
+        <v>-84.399850092273681</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>33.777161074810522</v>
+        <v>33.77801490203202</v>
       </c>
       <c r="B7" s="0">
-        <v>-84.399973115906874</v>
+        <v>-84.399895660622136</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0">
+        <v>33.778015566528744</v>
+      </c>
+      <c r="B8" s="0">
+        <v>-84.399820512819417</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0">
+        <v>33.778034836931781</v>
+      </c>
+      <c r="B9" s="0">
+        <v>-84.399835702268902</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0">
+        <v>33.778028856462335</v>
+      </c>
+      <c r="B10" s="0">
+        <v>-84.399836501713622</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0">
+        <v>33.777994967127611</v>
+      </c>
+      <c r="B11" s="0">
+        <v>-84.39983890004774</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0">
+        <v>33.777650092546949</v>
+      </c>
+      <c r="B12" s="0">
+        <v>-84.399848493384255</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added red cluster detection
</commit_message>
<xml_diff>
--- a/track-map/sample.xlsx
+++ b/track-map/sample.xlsx
@@ -20,9 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>latitudelongitude</t>
+  </si>
+  <si>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>longitude</t>
   </si>
   <si>
     <t>latitude</t>
@@ -163,7 +169,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="64">
+  <borders count="67">
     <border>
       <left/>
       <right/>
@@ -234,11 +240,14 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -303,6 +312,9 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="61" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="62" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="63" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="64" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="65" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="66" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -631,98 +643,98 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>33.77757633306333</v>
+        <v>33.777851435678905</v>
       </c>
       <c r="B2" s="0">
-        <v>-84.399890863953885</v>
+        <v>-84.399818913930005</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>33.777620190061235</v>
+        <v>33.777786979348228</v>
       </c>
       <c r="B3" s="0">
-        <v>-84.399819713374711</v>
+        <v>-84.399772546136845</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>33.777615538562522</v>
+        <v>33.777774353875714</v>
       </c>
       <c r="B4" s="0">
-        <v>-84.399861284499607</v>
+        <v>-84.399863682833754</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>33.777547759552618</v>
+        <v>33.777802927310852</v>
       </c>
       <c r="B5" s="0">
-        <v>-84.399821312264123</v>
+        <v>-84.399912448961047</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>33.777569023561483</v>
+        <v>33.777800933815683</v>
       </c>
       <c r="B6" s="0">
-        <v>-84.399850092273681</v>
+        <v>-84.399808521148785</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>33.77801490203202</v>
+        <v>33.777852764674911</v>
       </c>
       <c r="B7" s="0">
-        <v>-84.399895660622136</v>
+        <v>-84.399802925035814</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>33.778015566528744</v>
+        <v>33.777951110321581</v>
       </c>
       <c r="B8" s="0">
-        <v>-84.399820512819417</v>
+        <v>-84.399796529478138</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>33.778034836931781</v>
+        <v>33.777989651152311</v>
       </c>
       <c r="B9" s="0">
-        <v>-84.399835702268902</v>
+        <v>-84.399902056179798</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>33.778028856462335</v>
+        <v>33.778012908541783</v>
       </c>
       <c r="B10" s="0">
-        <v>-84.399836501713622</v>
+        <v>-84.399859685610195</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>33.777994967127611</v>
+        <v>33.77804413988342</v>
       </c>
       <c r="B11" s="0">
-        <v>-84.39983890004774</v>
+        <v>-84.399819713374711</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>33.777650092546949</v>
+        <v>33.778108596020594</v>
       </c>
       <c r="B12" s="0">
-        <v>-84.399848493384255</v>
+        <v>-84.399807721704065</v>
       </c>
     </row>
   </sheetData>

</xml_diff>